<commit_message>
renamed project from sphr to phr
</commit_message>
<xml_diff>
--- a/public/CodeSystem-apple-health-kit-biological-sex-code-system.xlsx
+++ b/public/CodeSystem-apple-health-kit-biological-sex-code-system.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/uv/sphr/CodeSystem/apple-health-kit-biological-sex-code-system</t>
+    <t>http://hl7.org/fhir/uv/phr/CodeSystem/apple-health-kit-biological-sex-code-system</t>
   </si>
   <si>
     <t>Version</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-11T01:07:49-06:00</t>
+    <t>2024-12-13T21:36:12-06:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>